<commit_message>
Revert "Sincro de comentarios"
This reverts commit bed83e4bae544210a12d946bd803e378865a9e02.
</commit_message>
<xml_diff>
--- a/Soporte/lista_paquetes_EHM.xlsx
+++ b/Soporte/lista_paquetes_EHM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AnacondaProjects\Project_TFM\IM_KS\Soporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="744">
   <si>
     <t>Name</t>
   </si>
@@ -2254,15 +2254,6 @@
   </si>
   <si>
     <t>4.5.0</t>
-  </si>
-  <si>
-    <t>pip install ipynb</t>
-  </si>
-  <si>
-    <t>Instalador</t>
-  </si>
-  <si>
-    <t>pip install metar</t>
   </si>
 </sst>
 </file>
@@ -3069,11 +3060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E336"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="A296" sqref="A296"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3082,7 +3072,7 @@
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3095,11 +3085,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3110,7 +3097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3121,7 +3108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3132,7 +3119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3143,7 +3130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3154,7 +3141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3165,7 +3152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3176,7 +3163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -3187,7 +3174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3198,7 +3185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3209,7 +3196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -3220,7 +3207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -3231,7 +3218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3242,7 +3229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -3256,7 +3243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -3267,7 +3254,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -3278,7 +3265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -3289,7 +3276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3300,7 +3287,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -3311,7 +3298,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -3322,7 +3309,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -3333,7 +3320,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -3344,7 +3331,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -3355,7 +3342,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -3380,7 +3367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -3391,7 +3378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -3402,7 +3389,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -3413,7 +3400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -3424,7 +3411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -3463,7 +3450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -3474,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -3485,7 +3472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -3496,7 +3483,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -3507,7 +3494,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -3518,7 +3505,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -3529,7 +3516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -3540,7 +3527,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -3551,7 +3538,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3562,7 +3549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -3573,7 +3560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>112</v>
       </c>
@@ -3584,7 +3571,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -3595,7 +3582,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>118</v>
       </c>
@@ -3606,7 +3593,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3617,7 +3604,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -3628,7 +3615,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -3639,7 +3626,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>128</v>
       </c>
@@ -3664,7 +3651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -3675,7 +3662,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>136</v>
       </c>
@@ -3686,7 +3673,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -3697,7 +3684,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>140</v>
       </c>
@@ -3708,7 +3695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>142</v>
       </c>
@@ -3719,7 +3706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -3730,7 +3717,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>146</v>
       </c>
@@ -3741,7 +3728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>148</v>
       </c>
@@ -3752,7 +3739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>150</v>
       </c>
@@ -3763,7 +3750,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>153</v>
       </c>
@@ -3774,7 +3761,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>156</v>
       </c>
@@ -3785,7 +3772,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>159</v>
       </c>
@@ -3810,7 +3797,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>165</v>
       </c>
@@ -3821,7 +3808,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>168</v>
       </c>
@@ -3846,7 +3833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>174</v>
       </c>
@@ -3885,7 +3872,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>180</v>
       </c>
@@ -3896,7 +3883,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -3921,7 +3908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>186</v>
       </c>
@@ -3932,7 +3919,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>188</v>
       </c>
@@ -3943,7 +3930,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>190</v>
       </c>
@@ -3968,7 +3955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -3993,7 +3980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>199</v>
       </c>
@@ -4004,7 +3991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>201</v>
       </c>
@@ -4015,7 +4002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>203</v>
       </c>
@@ -4040,7 +4027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>209</v>
       </c>
@@ -4051,7 +4038,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>212</v>
       </c>
@@ -4062,7 +4049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>214</v>
       </c>
@@ -4073,7 +4060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>215</v>
       </c>
@@ -4084,7 +4071,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>218</v>
       </c>
@@ -4095,7 +4082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>220</v>
       </c>
@@ -4106,7 +4093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>222</v>
       </c>
@@ -4116,11 +4103,8 @@
       <c r="C90" t="s">
         <v>224</v>
       </c>
-      <c r="D90" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>225</v>
       </c>
@@ -4131,7 +4115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>227</v>
       </c>
@@ -4142,7 +4126,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>229</v>
       </c>
@@ -4153,7 +4137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>231</v>
       </c>
@@ -4164,7 +4148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>233</v>
       </c>
@@ -4175,7 +4159,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>236</v>
       </c>
@@ -4186,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>238</v>
       </c>
@@ -4197,7 +4181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>240</v>
       </c>
@@ -4208,7 +4192,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>243</v>
       </c>
@@ -4247,7 +4231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>251</v>
       </c>
@@ -4258,7 +4242,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>253</v>
       </c>
@@ -4269,7 +4253,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>255</v>
       </c>
@@ -4280,7 +4264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>257</v>
       </c>
@@ -4319,7 +4303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>264</v>
       </c>
@@ -4372,7 +4356,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>271</v>
       </c>
@@ -4383,7 +4367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>273</v>
       </c>
@@ -4408,7 +4392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>278</v>
       </c>
@@ -4419,7 +4403,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>281</v>
       </c>
@@ -4472,7 +4456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>293</v>
       </c>
@@ -4483,7 +4467,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>296</v>
       </c>
@@ -4536,7 +4520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>303</v>
       </c>
@@ -4603,7 +4587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>317</v>
       </c>
@@ -4614,7 +4598,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>320</v>
       </c>
@@ -4653,7 +4637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>327</v>
       </c>
@@ -4664,7 +4648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>329</v>
       </c>
@@ -4675,7 +4659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>330</v>
       </c>
@@ -4686,7 +4670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>332</v>
       </c>
@@ -4697,7 +4681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>334</v>
       </c>
@@ -4708,7 +4692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>335</v>
       </c>
@@ -4719,7 +4703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>336</v>
       </c>
@@ -4730,7 +4714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>337</v>
       </c>
@@ -4741,7 +4725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>338</v>
       </c>
@@ -4752,7 +4736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>339</v>
       </c>
@@ -4763,7 +4747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>340</v>
       </c>
@@ -4774,7 +4758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>342</v>
       </c>
@@ -4785,7 +4769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>344</v>
       </c>
@@ -4796,7 +4780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>346</v>
       </c>
@@ -4807,7 +4791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>348</v>
       </c>
@@ -4818,7 +4802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>350</v>
       </c>
@@ -4829,7 +4813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>352</v>
       </c>
@@ -4840,7 +4824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>354</v>
       </c>
@@ -4851,7 +4835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>355</v>
       </c>
@@ -4862,7 +4846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>357</v>
       </c>
@@ -4873,7 +4857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>359</v>
       </c>
@@ -4884,7 +4868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>360</v>
       </c>
@@ -4895,7 +4879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>362</v>
       </c>
@@ -4906,7 +4890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>364</v>
       </c>
@@ -4917,7 +4901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>365</v>
       </c>
@@ -4928,7 +4912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>367</v>
       </c>
@@ -4939,7 +4923,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>370</v>
       </c>
@@ -4950,7 +4934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>372</v>
       </c>
@@ -4961,7 +4945,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>374</v>
       </c>
@@ -4975,7 +4959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>377</v>
       </c>
@@ -4986,7 +4970,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>380</v>
       </c>
@@ -4997,7 +4981,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>382</v>
       </c>
@@ -5010,11 +4994,8 @@
       <c r="D165" t="s">
         <v>384</v>
       </c>
-      <c r="E165" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>385</v>
       </c>
@@ -5025,7 +5006,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>387</v>
       </c>
@@ -5036,7 +5017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>389</v>
       </c>
@@ -5047,7 +5028,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>392</v>
       </c>
@@ -5058,7 +5039,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>394</v>
       </c>
@@ -5069,7 +5050,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>396</v>
       </c>
@@ -5080,7 +5061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>398</v>
       </c>
@@ -5091,7 +5072,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>400</v>
       </c>
@@ -5102,7 +5083,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>403</v>
       </c>
@@ -5113,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>404</v>
       </c>
@@ -5124,7 +5105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>406</v>
       </c>
@@ -5135,7 +5116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>407</v>
       </c>
@@ -5146,7 +5127,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>410</v>
       </c>
@@ -5157,7 +5138,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>412</v>
       </c>
@@ -5168,7 +5149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>413</v>
       </c>
@@ -5179,7 +5160,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>416</v>
       </c>
@@ -5190,7 +5171,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>419</v>
       </c>
@@ -5201,7 +5182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>421</v>
       </c>
@@ -5212,7 +5193,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>424</v>
       </c>
@@ -5223,7 +5204,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>427</v>
       </c>
@@ -5234,7 +5215,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>429</v>
       </c>
@@ -5245,7 +5226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>431</v>
       </c>
@@ -5256,7 +5237,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>433</v>
       </c>
@@ -5267,7 +5248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>435</v>
       </c>
@@ -5278,7 +5259,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>438</v>
       </c>
@@ -5289,7 +5270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>439</v>
       </c>
@@ -5300,7 +5281,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>442</v>
       </c>
@@ -5311,7 +5292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>444</v>
       </c>
@@ -5322,7 +5303,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>446</v>
       </c>
@@ -5333,7 +5314,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>449</v>
       </c>
@@ -5344,7 +5325,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>452</v>
       </c>
@@ -5355,7 +5336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>454</v>
       </c>
@@ -5366,7 +5347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>455</v>
       </c>
@@ -5377,7 +5358,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>458</v>
       </c>
@@ -5388,7 +5369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>460</v>
       </c>
@@ -5399,7 +5380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>462</v>
       </c>
@@ -5424,7 +5405,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>464</v>
       </c>
@@ -5435,7 +5416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>466</v>
       </c>
@@ -5446,7 +5427,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>469</v>
       </c>
@@ -5457,7 +5438,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>472</v>
       </c>
@@ -5468,7 +5449,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>472</v>
       </c>
@@ -5479,7 +5460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>475</v>
       </c>
@@ -5490,7 +5471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>477</v>
       </c>
@@ -5501,7 +5482,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>479</v>
       </c>
@@ -5512,7 +5493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>481</v>
       </c>
@@ -5523,7 +5504,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>484</v>
       </c>
@@ -5534,7 +5515,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>485</v>
       </c>
@@ -5545,7 +5526,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>487</v>
       </c>
@@ -5570,7 +5551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>490</v>
       </c>
@@ -5581,7 +5562,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>493</v>
       </c>
@@ -5592,7 +5573,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>496</v>
       </c>
@@ -5603,7 +5584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>498</v>
       </c>
@@ -5614,7 +5595,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>501</v>
       </c>
@@ -5625,7 +5606,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>504</v>
       </c>
@@ -5636,7 +5617,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>507</v>
       </c>
@@ -5647,7 +5628,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>510</v>
       </c>
@@ -5658,7 +5639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>512</v>
       </c>
@@ -5669,7 +5650,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>512</v>
       </c>
@@ -5680,7 +5661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>515</v>
       </c>
@@ -5691,7 +5672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>517</v>
       </c>
@@ -5702,7 +5683,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>520</v>
       </c>
@@ -5727,7 +5708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>524</v>
       </c>
@@ -5738,7 +5719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>526</v>
       </c>
@@ -5749,7 +5730,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>529</v>
       </c>
@@ -5760,7 +5741,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>531</v>
       </c>
@@ -5771,7 +5752,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>533</v>
       </c>
@@ -5810,7 +5791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>539</v>
       </c>
@@ -5835,7 +5816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>544</v>
       </c>
@@ -5846,7 +5827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>546</v>
       </c>
@@ -5857,7 +5838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>548</v>
       </c>
@@ -5868,7 +5849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>550</v>
       </c>
@@ -5879,7 +5860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>552</v>
       </c>
@@ -5890,7 +5871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>553</v>
       </c>
@@ -5901,7 +5882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>554</v>
       </c>
@@ -5912,7 +5893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>556</v>
       </c>
@@ -5923,7 +5904,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>559</v>
       </c>
@@ -5934,7 +5915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>561</v>
       </c>
@@ -5945,7 +5926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>562</v>
       </c>
@@ -5956,7 +5937,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>564</v>
       </c>
@@ -5967,7 +5948,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>566</v>
       </c>
@@ -5978,7 +5959,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>567</v>
       </c>
@@ -5989,7 +5970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>568</v>
       </c>
@@ -6028,7 +6009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>576</v>
       </c>
@@ -6039,7 +6020,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>579</v>
       </c>
@@ -6050,7 +6031,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>582</v>
       </c>
@@ -6061,7 +6042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>584</v>
       </c>
@@ -6072,7 +6053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>585</v>
       </c>
@@ -6097,7 +6078,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>589</v>
       </c>
@@ -6108,7 +6089,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>592</v>
       </c>
@@ -6119,7 +6100,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>594</v>
       </c>
@@ -6130,7 +6111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>596</v>
       </c>
@@ -6141,7 +6122,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>598</v>
       </c>
@@ -6166,7 +6147,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>603</v>
       </c>
@@ -6177,7 +6158,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>605</v>
       </c>
@@ -6188,7 +6169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>606</v>
       </c>
@@ -6199,7 +6180,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>608</v>
       </c>
@@ -6210,7 +6191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>610</v>
       </c>
@@ -6221,7 +6202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>611</v>
       </c>
@@ -6232,7 +6213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>612</v>
       </c>
@@ -6243,7 +6224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>614</v>
       </c>
@@ -6254,7 +6235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>615</v>
       </c>
@@ -6265,7 +6246,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>618</v>
       </c>
@@ -6276,7 +6257,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>620</v>
       </c>
@@ -6287,7 +6268,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>622</v>
       </c>
@@ -6312,7 +6293,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>627</v>
       </c>
@@ -6323,7 +6304,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>629</v>
       </c>
@@ -6334,7 +6315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>630</v>
       </c>
@@ -6345,7 +6326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>632</v>
       </c>
@@ -6356,7 +6337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>634</v>
       </c>
@@ -6367,7 +6348,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>636</v>
       </c>
@@ -6378,7 +6359,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>638</v>
       </c>
@@ -6389,7 +6370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>640</v>
       </c>
@@ -6414,7 +6395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>646</v>
       </c>
@@ -6425,7 +6406,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>648</v>
       </c>
@@ -6436,7 +6417,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>651</v>
       </c>
@@ -6447,7 +6428,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>654</v>
       </c>
@@ -6458,7 +6439,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>654</v>
       </c>
@@ -6469,7 +6450,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>656</v>
       </c>
@@ -6480,7 +6461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>657</v>
       </c>
@@ -6491,7 +6472,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>659</v>
       </c>
@@ -6502,7 +6483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>661</v>
       </c>
@@ -6513,7 +6494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>662</v>
       </c>
@@ -6566,7 +6547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>674</v>
       </c>
@@ -6577,7 +6558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>675</v>
       </c>
@@ -6588,7 +6569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>677</v>
       </c>
@@ -6599,7 +6580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>679</v>
       </c>
@@ -6610,7 +6591,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>682</v>
       </c>
@@ -6621,7 +6602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>683</v>
       </c>
@@ -6632,7 +6613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>685</v>
       </c>
@@ -6643,7 +6624,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>688</v>
       </c>
@@ -6654,7 +6635,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>688</v>
       </c>
@@ -6665,7 +6646,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>692</v>
       </c>
@@ -6676,7 +6657,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>694</v>
       </c>
@@ -6687,7 +6668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>696</v>
       </c>
@@ -6698,7 +6679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>698</v>
       </c>
@@ -6709,7 +6690,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>701</v>
       </c>
@@ -6720,7 +6701,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>703</v>
       </c>
@@ -6745,7 +6726,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>704</v>
       </c>
@@ -6756,7 +6737,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>707</v>
       </c>
@@ -6767,7 +6748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>709</v>
       </c>
@@ -6778,7 +6759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>711</v>
       </c>
@@ -6789,7 +6770,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>713</v>
       </c>
@@ -6800,7 +6781,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>715</v>
       </c>
@@ -6811,7 +6792,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>717</v>
       </c>
@@ -6822,7 +6803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>719</v>
       </c>
@@ -6833,7 +6814,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>722</v>
       </c>
@@ -6844,7 +6825,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>724</v>
       </c>
@@ -6855,7 +6836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>726</v>
       </c>
@@ -6866,7 +6847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>728</v>
       </c>
@@ -6905,7 +6886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>736</v>
       </c>
@@ -6930,7 +6911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>741</v>
       </c>
@@ -6941,7 +6922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>742</v>
       </c>
@@ -6953,7 +6934,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D336"/>
+  <autoFilter ref="A1:D336">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>